<commit_message>
modelling and add documents
</commit_message>
<xml_diff>
--- a/documents/excel/pembelian 10-06-2023.xlsx
+++ b/documents/excel/pembelian 10-06-2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kuliah\semester8\tugas akhir\project_skripsi\documents\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4BEF32-6F43-4F0E-AE57-44F9E2487F27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B4815F-08C0-4BE8-8EBF-557A8DADCF0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{B701851D-CDCB-45C2-9847-518B7740095D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>no</t>
   </si>
@@ -167,21 +167,12 @@
     <t>Natrium Karbonat</t>
   </si>
   <si>
-    <t>Wavemaker</t>
-  </si>
-  <si>
-    <t>Amara</t>
-  </si>
-  <si>
     <t>Zoanthus</t>
   </si>
   <si>
     <t>none</t>
   </si>
   <si>
-    <t>Alat tes Alkalinity</t>
-  </si>
-  <si>
     <t xml:space="preserve">Salifert </t>
   </si>
   <si>
@@ -189,6 +180,33 @@
   </si>
   <si>
     <t>Alat tes Magnesium</t>
+  </si>
+  <si>
+    <t>Box Panel Listrik Outdoor Topi 30x40x20</t>
+  </si>
+  <si>
+    <t>Akrilik</t>
+  </si>
+  <si>
+    <t>Printer Epson L121 A4 Ink Tank</t>
+  </si>
+  <si>
+    <t>Epson</t>
+  </si>
+  <si>
+    <t>Wavemaker AAWM8000</t>
+  </si>
+  <si>
+    <t>Recent</t>
+  </si>
+  <si>
+    <t>Kertas Hvs Paper One A4 80 gram</t>
+  </si>
+  <si>
+    <t>PaperOne</t>
+  </si>
+  <si>
+    <t>Alat tes Alkalinity (ion karbonat)</t>
   </si>
 </sst>
 </file>
@@ -298,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -315,9 +333,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -341,9 +356,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -357,11 +369,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -678,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D99DD1A-5073-4A13-987E-AAE684E69373}">
-  <dimension ref="B2:H44"/>
+  <dimension ref="B2:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +706,7 @@
     <col min="2" max="2" width="3.28515625" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -964,7 +981,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -982,7 +999,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -1000,7 +1017,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -1018,7 +1035,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -1036,7 +1053,7 @@
         <v>19800</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -1054,26 +1071,26 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="4">
         <f>SUM(F3:F21)</f>
         <v>293660</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E25" s="5" t="s">
@@ -1086,289 +1103,369 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="18">
-        <v>1</v>
-      </c>
-      <c r="C26" s="18" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="16">
+        <v>1</v>
+      </c>
+      <c r="C26" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="20">
+      <c r="E26" s="18">
         <v>99000</v>
       </c>
-      <c r="F26" s="21">
-        <v>1</v>
-      </c>
-      <c r="G26" s="20">
+      <c r="F26" s="19">
+        <v>1</v>
+      </c>
+      <c r="G26" s="18">
         <f>(E26*F26)</f>
         <v>99000</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="18">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="16">
         <v>2</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="20">
+      <c r="E27" s="18">
         <v>85000</v>
       </c>
-      <c r="F27" s="21">
-        <v>1</v>
-      </c>
-      <c r="G27" s="20">
-        <f t="shared" ref="G27:G44" si="4">(E27*F27)</f>
+      <c r="F27" s="19">
+        <v>1</v>
+      </c>
+      <c r="G27" s="18">
+        <f t="shared" ref="G27:G38" si="4">(E27*F27)</f>
         <v>85000</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="18">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="16">
         <v>3</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="20">
+      <c r="E28" s="18">
         <v>85000</v>
       </c>
-      <c r="F28" s="21">
-        <v>1</v>
-      </c>
-      <c r="G28" s="20">
+      <c r="F28" s="19">
+        <v>1</v>
+      </c>
+      <c r="G28" s="18">
         <f t="shared" si="4"/>
         <v>85000</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="18">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="16">
         <v>4</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E29" s="18">
         <v>85000</v>
       </c>
-      <c r="F29" s="21">
-        <v>1</v>
-      </c>
-      <c r="G29" s="20">
+      <c r="F29" s="19">
+        <v>1</v>
+      </c>
+      <c r="G29" s="18">
         <f t="shared" si="4"/>
         <v>85000</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="18">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="16">
         <v>5</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="18">
+        <v>90000</v>
+      </c>
+      <c r="F30" s="19">
+        <v>2</v>
+      </c>
+      <c r="G30" s="21">
+        <f t="shared" si="4"/>
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="16">
+        <v>6</v>
+      </c>
+      <c r="C31" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D31" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="20">
-        <v>65000</v>
-      </c>
-      <c r="F30" s="21">
-        <v>2</v>
-      </c>
-      <c r="G30" s="24">
-        <f t="shared" si="4"/>
-        <v>130000</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="18">
-        <v>6</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" s="20">
+      <c r="E31" s="18">
         <v>112000</v>
       </c>
-      <c r="F31" s="21">
-        <v>1</v>
-      </c>
-      <c r="G31" s="20">
+      <c r="F31" s="19">
+        <v>1</v>
+      </c>
+      <c r="G31" s="18">
         <f t="shared" si="4"/>
         <v>112000</v>
       </c>
-      <c r="H31" s="22">
-        <f>SUM(G26:G31)</f>
-        <v>596000</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="13">
+    </row>
+    <row r="32" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="12">
         <v>7</v>
       </c>
-      <c r="C32" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E32" s="7">
+      <c r="C32" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="6">
         <v>140000</v>
       </c>
-      <c r="F32" s="15">
-        <v>1</v>
-      </c>
-      <c r="G32" s="17">
+      <c r="F32" s="14">
+        <v>1</v>
+      </c>
+      <c r="G32" s="15">
         <f t="shared" si="4"/>
         <v>140000</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="13">
+      <c r="B33" s="12">
         <v>8</v>
       </c>
-      <c r="C33" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" s="7">
+      <c r="C33" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="6">
         <v>220000</v>
       </c>
-      <c r="F33" s="15">
-        <v>1</v>
-      </c>
-      <c r="G33" s="7">
+      <c r="F33" s="14">
+        <v>1</v>
+      </c>
+      <c r="G33" s="6">
         <f t="shared" si="4"/>
         <v>220000</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="13">
+      <c r="B34" s="12">
         <v>9</v>
       </c>
-      <c r="C34" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" s="7">
+      <c r="C34" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="6">
         <v>220000</v>
       </c>
-      <c r="F34" s="15">
-        <v>1</v>
-      </c>
-      <c r="G34" s="7">
+      <c r="F34" s="14">
+        <v>1</v>
+      </c>
+      <c r="G34" s="6">
         <f t="shared" si="4"/>
         <v>220000</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="s">
+    <row r="35" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="16">
+        <v>10</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="18">
+        <v>155000</v>
+      </c>
+      <c r="F35" s="19">
+        <v>1</v>
+      </c>
+      <c r="G35" s="18">
+        <f t="shared" si="4"/>
+        <v>155000</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="16">
+        <v>11</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="18">
+        <v>15000</v>
+      </c>
+      <c r="F36" s="19">
+        <v>1</v>
+      </c>
+      <c r="G36" s="18">
+        <f t="shared" si="4"/>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="16">
+        <v>12</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="18">
+        <v>1758000</v>
+      </c>
+      <c r="F37" s="19">
+        <v>1</v>
+      </c>
+      <c r="G37" s="18">
+        <f t="shared" si="4"/>
+        <v>1758000</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="16">
+        <v>13</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="18">
+        <v>46000</v>
+      </c>
+      <c r="F38" s="19">
+        <v>1</v>
+      </c>
+      <c r="G38" s="18">
+        <f t="shared" si="4"/>
+        <v>46000</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="16">
-        <f>SUM(G26:G44)</f>
-        <v>1176000</v>
-      </c>
-      <c r="G35" s="16"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="11"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="11"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="11"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="11"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="23">
+        <f>SUM(G26:G38)</f>
+        <v>3200000</v>
+      </c>
+      <c r="G39" s="23"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="11"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="10"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="11"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="10"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="11"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="10"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="11"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="10"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="11"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="10"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F39:G39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>